<commit_message>
Add exception handling, configure error logging
</commit_message>
<xml_diff>
--- a/surveyapp/data/all_users.xlsx
+++ b/surveyapp/data/all_users.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>first_name</t>
   </si>
@@ -34,28 +34,16 @@
     <t>survey_done</t>
   </si>
   <si>
-    <t>Natalija</t>
-  </si>
-  <si>
     <t>Aleksandar</t>
   </si>
   <si>
     <t>Gajic</t>
   </si>
   <si>
-    <t>2023_07_11_21_27_31</t>
-  </si>
-  <si>
-    <t>2023_07_11_21_31_34</t>
-  </si>
-  <si>
-    <t>nat.gaj98@gmail.com</t>
+    <t>2023_07_12_10_36_02</t>
   </si>
   <si>
     <t>gajic7080@gmail.com</t>
-  </si>
-  <si>
-    <t>1lbCvs1hADW3mD5c66mzpqb7ziKmDGtr5QoGX7pISYs</t>
   </si>
   <si>
     <t>Qmi9nT6p5G-tm03YAAsHhCaf_5XHOwXocy9IiDPYSKc</t>
@@ -416,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -447,39 +435,19 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>